<commit_message>
AE-1396: new pom extraction mojo
- added relationship tracking to new mojo
- introduced relationship registry to core
- remove old relationship tracker
- moved inventory separator from old relationship tracking to new registry
- added tests
</commit_message>
<xml_diff>
--- a/libraries/ae-inventory-processor/src/test/resources/separator/keycloak-25.0.4.xlsx
+++ b/libraries/ae-inventory-processor/src/test/resources/separator/keycloak-25.0.4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfuegen/IdeaProjects/metaeffekt-core/libraries/ae-inventory-processor/src/test/resources/separator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FAD24F-4595-4C4B-873E-38F0575C32FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27B8E5E-BF7B-634B-8FD3-AFB458AF4C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67200" windowHeight="44300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34460" yWindow="620" windowWidth="34220" windowHeight="28060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Artifacts" sheetId="1" r:id="rId1"/>
@@ -8921,7 +8921,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -8934,6 +8934,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9272,8 +9275,8 @@
   <dimension ref="A1:X451"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <pane ySplit="1" topLeftCell="A386" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C432" sqref="C432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9307,7 +9310,7 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -9389,8 +9392,39 @@
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="A3" t="s">
+        <v>2684</v>
+      </c>
+      <c r="D3" t="s">
+        <v>857</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1474</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2685</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" t="s">
+        <v>2685</v>
+      </c>
+      <c r="W3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -27665,39 +27699,8 @@
       </c>
     </row>
     <row r="437" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A437" t="s">
-        <v>2684</v>
-      </c>
-      <c r="D437" t="s">
-        <v>857</v>
-      </c>
-      <c r="E437" t="s">
-        <v>1473</v>
-      </c>
-      <c r="F437" t="s">
-        <v>1474</v>
-      </c>
-      <c r="G437" t="s">
-        <v>2685</v>
-      </c>
-      <c r="I437" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N437" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O437" t="s">
-        <v>30</v>
-      </c>
-      <c r="T437" t="s">
-        <v>39</v>
-      </c>
-      <c r="U437" t="s">
-        <v>2685</v>
-      </c>
-      <c r="W437" t="s">
-        <v>33</v>
-      </c>
+      <c r="I437" s="4"/>
+      <c r="N437" s="4"/>
     </row>
     <row r="438" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
@@ -28199,9 +28202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AV9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O25" sqref="O25"/>
+      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>